<commit_message>
V0.1 main_file (P04_01_notebook): - EDA done (can be improved) - Feature engenering / selection Partially done - Clean done (can be improved by outlier deep clean) Other_file (merge_file): - EDA all file in progress - feature engenering / selection in progress - clean to do
Added files description
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_4\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625F7274-73C2-4B32-AA79-3EFF0764CCC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE019439-081D-4F94-8443-70D4F67322C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>la variable cible a été identifiée</t>
+  </si>
+  <si>
+    <t>Regrouper les fichier en 1 fichier à analyser ?</t>
+  </si>
+  <si>
+    <t>Revoir la standartisation avant la séparation pour l'implementer dans une pipline</t>
+  </si>
+  <si>
+    <t>Faire labelEncoder pour les variable binaire</t>
+  </si>
+  <si>
+    <t>Revoir la méthode peux être améliorer</t>
   </si>
 </sst>
 </file>
@@ -474,26 +486,26 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -778,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -803,10 +815,10 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="39" customHeight="1" thickBot="1">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
@@ -814,9 +826,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17"/>
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
@@ -826,12 +840,14 @@
         <v>5</v>
       </c>
       <c r="C6" s="10">
-        <v>0</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="F6" s="8">
-        <f>AVERAGE(C5:C11,C13:C16,C18:C22)</f>
-        <v>0</v>
+        <f>AVERAGE(C5:C11,C13:C16,C18:C22,C24:C26)</f>
+        <v>0.54736842105263162</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1">
@@ -839,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="14"/>
     </row>
@@ -848,16 +864,18 @@
         <v>7</v>
       </c>
       <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="D8" s="15"/>
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="2:8" ht="43.5" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="10">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="14"/>
     </row>
@@ -866,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D10" s="15"/>
     </row>
@@ -875,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="19"/>
       <c r="F11" s="5"/>
@@ -883,10 +901,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="18"/>
     </row>
     <row r="13" spans="2:8" ht="40.5" customHeight="1">
@@ -894,7 +912,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="17"/>
     </row>
@@ -903,16 +921,18 @@
         <v>11</v>
       </c>
       <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="15"/>
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="40.5" customHeight="1">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D15" s="14"/>
     </row>
@@ -921,15 +941,15 @@
         <v>12</v>
       </c>
       <c r="C16" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="18"/>
     </row>
     <row r="18" spans="2:4" ht="65.5" customHeight="1">
@@ -937,7 +957,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="17"/>
     </row>
@@ -946,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="10">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D19" s="15"/>
     </row>
@@ -955,7 +975,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="10">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D20" s="14"/>
     </row>
@@ -964,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D21" s="15"/>
     </row>
@@ -973,15 +993,15 @@
         <v>18</v>
       </c>
       <c r="C22" s="13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D22" s="16"/>
     </row>
     <row r="23" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="18"/>
     </row>
     <row r="24" spans="2:4" ht="42.5" customHeight="1">
@@ -989,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="14"/>
     </row>
@@ -1012,7 +1032,7 @@
       <c r="D26" s="16"/>
     </row>
     <row r="27" spans="2:4" ht="27.5" customHeight="1">
-      <c r="B27" s="26"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="10"/>
     </row>
     <row r="28" spans="2:4" ht="27.5" customHeight="1" thickBot="1">
@@ -1028,18 +1048,8 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B23:C23"/>
   </mergeCells>
-  <conditionalFormatting sqref="C18:C22 C5:C11 C13:C16">
+  <conditionalFormatting sqref="C18:C22 C5:C11 C13:C16 C24:C26">
     <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color theme="5"/>
-        <color theme="9"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:C28">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>

</xml_diff>

<commit_message>
V0.5 : modeling and optimisation for random forest only, try other model juste with started data clean. Todo : - Create Pipeline for all model try to optimise and test quickly - review method under_sampling to weight_balance
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_4\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE019439-081D-4F94-8443-70D4F67322C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CCED1A-035E-4203-8E2F-DCCF5AEE258C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -120,13 +120,22 @@
     <t>Regrouper les fichier en 1 fichier à analyser ?</t>
   </si>
   <si>
-    <t>Revoir la standartisation avant la séparation pour l'implementer dans une pipline</t>
-  </si>
-  <si>
-    <t>Faire labelEncoder pour les variable binaire</t>
-  </si>
-  <si>
-    <t>Revoir la méthode peux être améliorer</t>
+    <t>Implémentation dans un pipline et peut-être revoir pour l'améliorer</t>
+  </si>
+  <si>
+    <t>Revoir la méthode peux être améliorer / pas nécessaire sur le random forest</t>
+  </si>
+  <si>
+    <t>Oui mais perfectible je pense</t>
+  </si>
+  <si>
+    <t>Fbeta avec beta = 2</t>
+  </si>
+  <si>
+    <t>max_depth principalement</t>
+  </si>
+  <si>
+    <t>Faire un test avec un CV ?</t>
   </si>
 </sst>
 </file>
@@ -790,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -826,7 +835,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="10">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>27</v>
@@ -840,14 +849,12 @@
         <v>5</v>
       </c>
       <c r="C6" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D6" s="15"/>
       <c r="F6" s="8">
         <f>AVERAGE(C5:C11,C13:C16,C18:C22,C24:C26)</f>
-        <v>0.54736842105263162</v>
+        <v>0.76578947368421058</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1">
@@ -859,15 +866,15 @@
       </c>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="43.5" customHeight="1">
+    <row r="8" spans="2:8" ht="56">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="43.5" customHeight="1">
@@ -875,16 +882,18 @@
         <v>8</v>
       </c>
       <c r="C9" s="10">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="43.5" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="10">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D10" s="15"/>
     </row>
@@ -893,7 +902,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="11">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D11" s="19"/>
       <c r="F11" s="5"/>
@@ -921,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="10">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>28</v>
@@ -932,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="10">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="D15" s="14"/>
     </row>
@@ -941,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D16" s="15"/>
     </row>
@@ -957,16 +966,18 @@
         <v>14</v>
       </c>
       <c r="C18" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="17"/>
+        <v>0.9</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="78" customHeight="1">
       <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="10">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D19" s="15"/>
     </row>
@@ -975,16 +986,18 @@
         <v>16</v>
       </c>
       <c r="C20" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="14"/>
+        <v>0.3</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="2:4" ht="55" customHeight="1">
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="10">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="15"/>
     </row>
@@ -993,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="13">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D22" s="16"/>
     </row>
@@ -1009,16 +1022,18 @@
         <v>19</v>
       </c>
       <c r="C24" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D24" s="14"/>
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="25" spans="2:4" ht="42.5" customHeight="1">
       <c r="B25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D25" s="15"/>
     </row>
@@ -1027,7 +1042,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D26" s="16"/>
     </row>

</xml_diff>

<commit_message>
update main file, and iteratif testing, not all finish in main fileall cells are not executed at the end
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_4\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CCED1A-035E-4203-8E2F-DCCF5AEE258C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4070A703-D1F2-46C6-BAB7-6026BB4088B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -120,22 +120,19 @@
     <t>Regrouper les fichier en 1 fichier à analyser ?</t>
   </si>
   <si>
-    <t>Implémentation dans un pipline et peut-être revoir pour l'améliorer</t>
-  </si>
-  <si>
-    <t>Revoir la méthode peux être améliorer / pas nécessaire sur le random forest</t>
-  </si>
-  <si>
-    <t>Oui mais perfectible je pense</t>
-  </si>
-  <si>
     <t>Fbeta avec beta = 2</t>
   </si>
   <si>
-    <t>max_depth principalement</t>
-  </si>
-  <si>
-    <t>Faire un test avec un CV ?</t>
+    <t>Fait dans une pipeline</t>
+  </si>
+  <si>
+    <t>GridSearch pour l'optimisation</t>
+  </si>
+  <si>
+    <t>Tableau à faire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHAP / LIME </t>
   </si>
 </sst>
 </file>
@@ -800,7 +797,7 @@
   <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -854,7 +851,7 @@
       <c r="D6" s="15"/>
       <c r="F6" s="8">
         <f>AVERAGE(C5:C11,C13:C16,C18:C22,C24:C26)</f>
-        <v>0.76578947368421058</v>
+        <v>0.96052631578947367</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1">
@@ -866,27 +863,23 @@
       </c>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="56">
+    <row r="8" spans="2:8" ht="28">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="2:8" ht="43.5" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:8" ht="43.5" customHeight="1">
       <c r="B10" s="4" t="s">
@@ -902,9 +895,11 @@
         <v>10</v>
       </c>
       <c r="C11" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
@@ -930,10 +925,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="10">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="40.5" customHeight="1">
@@ -966,10 +961,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="12">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="78" customHeight="1">
@@ -986,10 +981,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="10">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="55" customHeight="1">
@@ -997,9 +992,11 @@
         <v>17</v>
       </c>
       <c r="C21" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D21" s="15"/>
+        <v>0.7</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="2:4" ht="45.5" customHeight="1" thickBot="1">
       <c r="B22" s="3" t="s">
@@ -1022,18 +1019,16 @@
         <v>19</v>
       </c>
       <c r="C24" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>32</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D24" s="14"/>
     </row>
     <row r="25" spans="2:4" ht="42.5" customHeight="1">
       <c r="B25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D25" s="15"/>
     </row>
@@ -1042,7 +1037,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D26" s="16"/>
     </row>

</xml_diff>

<commit_message>
V1.0, final version submited to OC
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_4\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4070A703-D1F2-46C6-BAB7-6026BB4088B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C90EAC8-F21B-490B-B0C7-7C38108B0132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,7 +797,7 @@
   <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -832,7 +832,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="10">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>27</v>
@@ -851,7 +851,7 @@
       <c r="D6" s="15"/>
       <c r="F6" s="8">
         <f>AVERAGE(C5:C11,C13:C16,C18:C22,C24:C26)</f>
-        <v>0.96052631578947367</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1">
@@ -925,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>29</v>
@@ -936,7 +936,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D15" s="14"/>
     </row>
@@ -981,7 +981,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="10">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>30</v>
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="10">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>31</v>

</xml_diff>